<commit_message>
update report and load, reload plan written but not tested
added printout test data for future reports
</commit_message>
<xml_diff>
--- a/Test Data/Printout Data/Printout_data_analysis.xlsx
+++ b/Test Data/Printout Data/Printout_data_analysis.xlsx
@@ -1,28 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://queensuca-my.sharepoint.com/personal/gs13_queensu_ca/Documents/Python/Projects/EclipseRelated/PlanEvaluation/Test Data/Printout Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="220" documentId="11_B836798684E48AABFDA164109C795CCD52C2B8D8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{54E5F8E6-0DEF-4162-B1B2-3172230DF649}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="17235" windowHeight="15600" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="points" sheetId="4" r:id="rId1"/>
     <sheet name="fields" sheetId="3" r:id="rId2"/>
     <sheet name="plan" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId4"/>
-    <sheet name="points (2)" sheetId="5" r:id="rId5"/>
-    <sheet name="fields (2)" sheetId="7" r:id="rId6"/>
+    <sheet name="points (2)" sheetId="5" r:id="rId4"/>
+    <sheet name="fields (2)" sheetId="7" r:id="rId5"/>
+    <sheet name="Variable Mapping" sheetId="8" r:id="rId6"/>
+    <sheet name="points (3)" sheetId="9" r:id="rId7"/>
+    <sheet name="fields (3)" sheetId="10" r:id="rId8"/>
+    <sheet name="plan (2)" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="206">
   <si>
     <t>PatientLastName</t>
   </si>
@@ -532,13 +549,121 @@
   </si>
   <si>
     <t>Difference</t>
+  </si>
+  <si>
+    <t>RefPoints</t>
+  </si>
+  <si>
+    <t>RefPointType</t>
+  </si>
+  <si>
+    <t>RefPointTotalDosePerFraction</t>
+  </si>
+  <si>
+    <t>RefPointTotalDose</t>
+  </si>
+  <si>
+    <t>IsPrimaryRefPoint</t>
+  </si>
+  <si>
+    <t>RefPointPatientVolumeId</t>
+  </si>
+  <si>
+    <t>FieldMachineModel</t>
+  </si>
+  <si>
+    <t>FieldMachineScale</t>
+  </si>
+  <si>
+    <t>FieldMonitorUnitsPerGy</t>
+  </si>
+  <si>
+    <t>FieldSymmetry</t>
+  </si>
+  <si>
+    <t>PatientMiddleName</t>
+  </si>
+  <si>
+    <t>PatientDateOfBirth</t>
+  </si>
+  <si>
+    <t>PrimaryOncologist</t>
+  </si>
+  <si>
+    <t>CurrentDateShort</t>
+  </si>
+  <si>
+    <t>ApplicationName</t>
+  </si>
+  <si>
+    <t>TaskName</t>
+  </si>
+  <si>
+    <t>TaskVersion</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>ImagingDeviceManufacturer</t>
+  </si>
+  <si>
+    <t>ImagingDeviceSerialNumber</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>d=9cm</t>
+  </si>
+  <si>
+    <t>d=6cm</t>
+  </si>
+  <si>
+    <t>d=3cm</t>
+  </si>
+  <si>
+    <t>Asymmetric X</t>
+  </si>
+  <si>
+    <t>Varian IEC</t>
+  </si>
+  <si>
+    <t>TDS</t>
+  </si>
+  <si>
+    <t>GE MEDICAL SYSTEMS</t>
+  </si>
+  <si>
+    <t>Friday, October 04, 2019 16</t>
+  </si>
+  <si>
+    <t>CCSEO at KGH, Kingston, ON</t>
+  </si>
+  <si>
+    <t>External Beam Planning</t>
+  </si>
+  <si>
+    <t>Efective Depth</t>
+  </si>
+  <si>
+    <t>Total Dose</t>
+  </si>
+  <si>
+    <t>Calculation Log</t>
+  </si>
+  <si>
+    <t>Field Name</t>
+  </si>
+  <si>
+    <t>MUs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,8 +679,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,8 +723,44 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -586,18 +777,132 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -613,12 +918,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="gsalomon" refreshedDate="43742.619090277774" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="40">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="gsalomon" refreshedDate="43742.619090277774" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="40" xr:uid="{00000000-000A-0000-FFFF-FFFF0A000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table15"/>
   </cacheSource>
@@ -1096,7 +1404,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="P3:T16" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
   <pivotFields count="8">
     <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -1265,97 +1573,100 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F41" totalsRowShown="0">
-  <autoFilter ref="A1:F41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F41" totalsRowShown="0">
+  <autoFilter ref="A1:F41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="FieldDose"/>
-    <tableColumn id="2" name="FieldRefPointEffectiveDepth"/>
-    <tableColumn id="3" name="FieldRefPointPointDepth"/>
-    <tableColumn id="4" name="FieldRefPointSSD"/>
-    <tableColumn id="5" name="RefPointId"/>
-    <tableColumn id="6" name="field_name"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FieldDose"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="FieldRefPointEffectiveDepth"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="FieldRefPointPointDepth"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FieldRefPointSSD"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="RefPointId"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="field_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="J1:M9" totalsRowShown="0">
-  <autoFilter ref="J1:M9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="J1:M9" totalsRowShown="0">
+  <autoFilter ref="J1:M9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="RefPointId"/>
-    <tableColumn id="2" name="RefPointX"/>
-    <tableColumn id="3" name="RefPointY"/>
-    <tableColumn id="4" name="RefPointZ"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="RefPointId"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="RefPointX"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="RefPointY"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="RefPointZ"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:AC5" totalsRowShown="0">
-  <autoFilter ref="A1:AC5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:AC5" totalsRowShown="0">
+  <autoFilter ref="A1:AC5" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="29">
-    <tableColumn id="1" name="Course"/>
-    <tableColumn id="2" name="PlanId"/>
-    <tableColumn id="3" name="FieldId"/>
-    <tableColumn id="4" name="FieldName"/>
-    <tableColumn id="5" name="FieldMachineId"/>
-    <tableColumn id="6" name="FieldEnergyMode"/>
-    <tableColumn id="7" name="FieldGantryAngle"/>
-    <tableColumn id="8" name="FieldCollimatorAngle"/>
-    <tableColumn id="9" name="FieldTableAngle"/>
-    <tableColumn id="10" name="X1"/>
-    <tableColumn id="11" name="X2"/>
-    <tableColumn id="12" name="Y1"/>
-    <tableColumn id="13" name="Y2"/>
-    <tableColumn id="14" name="FieldIsocentreX"/>
-    <tableColumn id="15" name="FieldIsocentreY"/>
-    <tableColumn id="16" name="FieldIsocentreZ"/>
-    <tableColumn id="17" name="FieldSAD"/>
-    <tableColumn id="18" name="FieldSSD"/>
-    <tableColumn id="19" name="FieldActualSSD"/>
-    <tableColumn id="20" name="FieldMonitorUnits"/>
-    <tableColumn id="21" name="FieldWeightFactor"/>
-    <tableColumn id="22" name="FieldRefDose"/>
-    <tableColumn id="23" name="FieldNormFactor"/>
-    <tableColumn id="24" name="FieldNormMethod"/>
-    <tableColumn id="25" name="FieldDoseRate"/>
-    <tableColumn id="26" name="FieldTechnique"/>
-    <tableColumn id="27" name="FieldIMRT"/>
-    <tableColumn id="28" name="FieldCalculationWarning"/>
-    <tableColumn id="29" name="FieldCalculationInfo"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Course"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="PlanId"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FieldId"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="FieldName"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="FieldMachineId"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="FieldEnergyMode"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="FieldGantryAngle"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="FieldCollimatorAngle"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="FieldTableAngle"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="X1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="X2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Y1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Y2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="FieldIsocentreX"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="FieldIsocentreY"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="FieldIsocentreZ"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="FieldSAD"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="FieldSSD"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="FieldActualSSD"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="FieldMonitorUnits"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="FieldWeightFactor"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="FieldRefDose"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="FieldNormFactor"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="FieldNormMethod"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0200-000019000000}" name="FieldDoseRate"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0200-00001A000000}" name="FieldTechnique"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0200-00001B000000}" name="FieldIMRT"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="FieldCalculationWarning"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0200-00001D000000}" name="FieldCalculationInfo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:H41" totalsRowShown="0">
-  <autoFilter ref="A1:H41"/>
-  <sortState ref="A2:H41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table15" displayName="Table15" ref="A1:H41" totalsRowShown="0">
+  <autoFilter ref="A1:H41" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H41">
     <sortCondition ref="E2:E41"/>
     <sortCondition ref="B2:B41"/>
     <sortCondition ref="D2:D41"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Dose"/>
-    <tableColumn id="3" name="Depth"/>
-    <tableColumn id="4" name="SSD"/>
-    <tableColumn id="5" name="Point"/>
-    <tableColumn id="6" name="Field"/>
-    <tableColumn id="7" name="Side">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Dose"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Depth"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="SSD"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Point"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Field"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Side">
       <calculatedColumnFormula>LEFT(Table15[[#This Row],[Point]],FIND(" ",Table15[[#This Row],[Point]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Field Side" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Field Side" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],[Field]],Table37[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Field SSD" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Field SSD" dataDxfId="0">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],[Field]],Table37[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1364,45 +1675,45 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="J1:M9" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table26" displayName="Table26" ref="J1:M9" totalsRowShown="0">
   <tableColumns count="4">
-    <tableColumn id="1" name="Point"/>
-    <tableColumn id="2" name="X"/>
-    <tableColumn id="3" name="Y"/>
-    <tableColumn id="4" name="Z"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Point"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="X"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Y"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Z"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table37" displayName="Table37" ref="A1:X5" totalsRowShown="0">
-  <autoFilter ref="A1:X5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table37" displayName="Table37" ref="A1:X5" totalsRowShown="0">
+  <autoFilter ref="A1:X5" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="24">
-    <tableColumn id="3" name="Field"/>
-    <tableColumn id="30" name="Field Side"/>
-    <tableColumn id="18" name="Field SSD"/>
-    <tableColumn id="1" name="Course"/>
-    <tableColumn id="2" name="Plan"/>
-    <tableColumn id="5" name="Machine"/>
-    <tableColumn id="6" name="Energy"/>
-    <tableColumn id="7" name="Gantry"/>
-    <tableColumn id="8" name="Collimator"/>
-    <tableColumn id="9" name="Couch"/>
-    <tableColumn id="10" name="X1"/>
-    <tableColumn id="11" name="X2"/>
-    <tableColumn id="12" name="Y1"/>
-    <tableColumn id="13" name="Y2"/>
-    <tableColumn id="14" name="Iso X"/>
-    <tableColumn id="15" name="Iso Y"/>
-    <tableColumn id="16" name="Iso Z"/>
-    <tableColumn id="17" name="SAD"/>
-    <tableColumn id="20" name="Mus"/>
-    <tableColumn id="21" name="Field Weight"/>
-    <tableColumn id="22" name="Field Dose"/>
-    <tableColumn id="23" name="Norm Factor"/>
-    <tableColumn id="26" name="Technique"/>
-    <tableColumn id="28" name="Warning"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Field"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0500-00001E000000}" name="Field Side"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0500-000012000000}" name="Field SSD"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Course"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Plan"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Machine"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Energy"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Gantry"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Collimator"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Couch"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="X1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="X2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="Y1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Y2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0500-00000E000000}" name="Iso X"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Iso Y"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Iso Z"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="SAD"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0500-000014000000}" name="Mus"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0500-000015000000}" name="Field Weight"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0500-000016000000}" name="Field Dose"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0500-000017000000}" name="Norm Factor"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0500-00001A000000}" name="Technique"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0500-00001C000000}" name="Warning"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1451,7 +1762,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1484,9 +1795,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1519,6 +1847,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1694,7 +2039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2580,11 +2925,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3050,11 +3395,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A22" sqref="A22:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3226,10 +3571,10 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="15" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3447,41 +3792,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="8" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.85546875" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U41"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5064,12 +5379,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5465,4 +5780,3333 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82BC1C4-DC38-43BD-B308-419C0C4E626C}">
+  <dimension ref="A1:P48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="str">
+        <f t="shared" ref="P1:P10" si="0">_xlfn.CONCAT("'",O1,"',")</f>
+        <v>'PatientId',</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("'",A2,"': ","'",B2,"',")</f>
+        <v>'field_name': 'Field',</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G33" si="1">_xlfn.CONCAT("'",E2,"': ","'",F2,"',")</f>
+        <v>'PlanId': 'Plan',</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" si="0"/>
+        <v>'ImageId',</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="1"/>
+        <v>'Course': 'Course',</v>
+      </c>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="0"/>
+        <v>'ImageName',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C14" si="2">_xlfn.CONCAT("'",A4,"': ","'",B4,"',")</f>
+        <v>'RefPointId': 'Point',</v>
+      </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldId': 'Field',</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="0"/>
+        <v>'ImageUserOrigin',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="2"/>
+        <v>'FieldDose': 'Dose',</v>
+      </c>
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldName': 'Field Name',</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="0"/>
+        <v>'PlanModificationDate',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldMachineId': 'Machine',</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="0"/>
+        <v>'StructureId',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="2"/>
+        <v>'FieldRefPointSSD': 'SSD',</v>
+      </c>
+      <c r="E7" t="s">
+        <v>176</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="0"/>
+        <v>'StructureName',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="2"/>
+        <v>'FieldRefPointPointDepth': 'Depth',</v>
+      </c>
+      <c r="E8" t="s">
+        <v>177</v>
+      </c>
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="0"/>
+        <v>'PlanNormValue',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="2"/>
+        <v>'FieldRefPointEffectiveDepth': 'Efective Depth',</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldEnergyMode': 'Energy',</v>
+      </c>
+      <c r="I9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="0"/>
+        <v>'PrescribedDose',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="2"/>
+        <v>'RefPointX': 'X',</v>
+      </c>
+      <c r="E10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldDoseRate': '',</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="0"/>
+        <v>'Fractions',</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="2"/>
+        <v>'RefPointY': 'Y',</v>
+      </c>
+      <c r="E11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldTechnique': 'Technique',</v>
+      </c>
+      <c r="I11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="2"/>
+        <v>'RefPointZ': 'Z',</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldMonitorUnits': 'Mus',</v>
+      </c>
+      <c r="I12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" t="s">
+        <v>178</v>
+      </c>
+      <c r="I13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13">
+        <v>0.25</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="2"/>
+        <v>'RefPointTotalDose': 'Total Dose',</v>
+      </c>
+      <c r="E14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldRefDose': 'Field Dose',</v>
+      </c>
+      <c r="I14" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14">
+        <v>100</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldSAD': 'SAD',</v>
+      </c>
+      <c r="I16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="L16" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldSSD': 'Field SSD',</v>
+      </c>
+      <c r="I17" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17">
+        <v>100</v>
+      </c>
+      <c r="L17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="L18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" t="str">
+        <f>_xlfn.CONCAT("'",A19,"',")</f>
+        <v>'Point',</v>
+      </c>
+      <c r="E19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>'X1': 'X1',</v>
+      </c>
+      <c r="L19" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" ref="B20:B22" si="3">_xlfn.CONCAT("'",A20,"',")</f>
+        <v>'X',</v>
+      </c>
+      <c r="E20" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>'X2': 'X2',</v>
+      </c>
+      <c r="L20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="3"/>
+        <v>'Y',</v>
+      </c>
+      <c r="E21" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>'Y1': 'Y1',</v>
+      </c>
+      <c r="L21" t="s">
+        <v>45</v>
+      </c>
+      <c r="M21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="3"/>
+        <v>'Z',</v>
+      </c>
+      <c r="E22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>'Y2': 'Y2',</v>
+      </c>
+      <c r="L22" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>179</v>
+      </c>
+      <c r="L23" t="s">
+        <v>22</v>
+      </c>
+      <c r="M23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldGantryAngle': 'Gantry',</v>
+      </c>
+      <c r="L24" t="s">
+        <v>26</v>
+      </c>
+      <c r="M24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldCollimatorAngle': 'Collimator',</v>
+      </c>
+      <c r="L25" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="14" t="str">
+        <f>LEFT(A26,FIND(" ",A26))</f>
+        <v xml:space="preserve">Thin </v>
+      </c>
+      <c r="E26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldTableAngle': 'Couch',</v>
+      </c>
+      <c r="L26" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldIsocentreX': 'Iso X',</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldIsocentreY': 'Iso Y',</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="M28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="9" t="str">
+        <f>LEFT(A29,FIND(" ",A29))</f>
+        <v xml:space="preserve">Thin </v>
+      </c>
+      <c r="E29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldIsocentreZ': 'Iso Z',</v>
+      </c>
+      <c r="L29" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>92</v>
+      </c>
+      <c r="L30" t="s">
+        <v>51</v>
+      </c>
+      <c r="M30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldNormFactor': 'Norm Factor',</v>
+      </c>
+      <c r="L31" t="s">
+        <v>53</v>
+      </c>
+      <c r="M31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldWeightFactor': 'Field Weight',</v>
+      </c>
+      <c r="L32" t="s">
+        <v>54</v>
+      </c>
+      <c r="M32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v>'FieldCalculationWarning': 'Warning',</v>
+      </c>
+      <c r="L33" t="s">
+        <v>55</v>
+      </c>
+      <c r="M33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" ref="B34:B45" si="4">_xlfn.CONCAT("'",A34,"',")</f>
+        <v>'Plan',</v>
+      </c>
+      <c r="E34" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" t="s">
+        <v>203</v>
+      </c>
+      <c r="L34" t="s">
+        <v>57</v>
+      </c>
+      <c r="M34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="4"/>
+        <v>'Course',</v>
+      </c>
+      <c r="L35" t="s">
+        <v>58</v>
+      </c>
+      <c r="M35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="4"/>
+        <v>'Field',</v>
+      </c>
+      <c r="L36" t="s">
+        <v>60</v>
+      </c>
+      <c r="M36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="4"/>
+        <v>'Field Name',</v>
+      </c>
+      <c r="L37" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="M37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="4"/>
+        <v>'Energy',</v>
+      </c>
+      <c r="L38" t="s">
+        <v>62</v>
+      </c>
+      <c r="M38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="4"/>
+        <v>'MUs',</v>
+      </c>
+      <c r="L39" t="s">
+        <v>64</v>
+      </c>
+      <c r="M39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="4"/>
+        <v>'Field Dose',</v>
+      </c>
+      <c r="L40" t="s">
+        <v>65</v>
+      </c>
+      <c r="M40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="4"/>
+        <v>'SAD',</v>
+      </c>
+      <c r="L41" t="s">
+        <v>66</v>
+      </c>
+      <c r="M41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="4"/>
+        <v>'Field SSD',</v>
+      </c>
+      <c r="L42" t="s">
+        <v>67</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="4"/>
+        <v>'Iso X',</v>
+      </c>
+      <c r="L43" t="s">
+        <v>68</v>
+      </c>
+      <c r="M43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="4"/>
+        <v>'Norm Factor',</v>
+      </c>
+      <c r="L44" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="M44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="4"/>
+        <v>'Field Weight',</v>
+      </c>
+      <c r="L45" t="s">
+        <v>71</v>
+      </c>
+      <c r="M45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L46" t="s">
+        <v>72</v>
+      </c>
+      <c r="M46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L47" t="s">
+        <v>73</v>
+      </c>
+      <c r="M47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L48" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9329D523-BF93-4A77-ACC4-E6815308A2E7}">
+  <dimension ref="A1:O56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N1" t="s">
+        <v>174</v>
+      </c>
+      <c r="O1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2">
+        <v>154.4</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3">
+        <v>136.1</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4">
+        <v>118.4</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5">
+        <v>106.4</v>
+      </c>
+      <c r="F5">
+        <v>97.1</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6">
+        <v>161.6</v>
+      </c>
+      <c r="F6">
+        <v>97.1</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7">
+        <v>142.1</v>
+      </c>
+      <c r="F7">
+        <v>97.1</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8">
+        <v>123.1</v>
+      </c>
+      <c r="F8">
+        <v>97.1</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9">
+        <v>48.1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10">
+        <v>156.6</v>
+      </c>
+      <c r="F10">
+        <v>100.2</v>
+      </c>
+      <c r="G10">
+        <v>2.9</v>
+      </c>
+      <c r="H10">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11">
+        <v>137.19999999999999</v>
+      </c>
+      <c r="F11">
+        <v>100.2</v>
+      </c>
+      <c r="G11">
+        <v>5.9</v>
+      </c>
+      <c r="H11">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12">
+        <v>118.9</v>
+      </c>
+      <c r="F12">
+        <v>100.2</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D13">
+        <v>101.2</v>
+      </c>
+      <c r="F13">
+        <v>97</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D14">
+        <v>88.9</v>
+      </c>
+      <c r="F14">
+        <v>97</v>
+      </c>
+      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15">
+        <v>77.2</v>
+      </c>
+      <c r="F15">
+        <v>97</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16">
+        <v>69.3</v>
+      </c>
+      <c r="F16">
+        <v>94.1</v>
+      </c>
+      <c r="G16">
+        <v>12</v>
+      </c>
+      <c r="H16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17">
+        <v>106.2</v>
+      </c>
+      <c r="F17">
+        <v>94.1</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18">
+        <v>93.1</v>
+      </c>
+      <c r="F18">
+        <v>94.1</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="F19">
+        <v>94.1</v>
+      </c>
+      <c r="G19">
+        <v>9</v>
+      </c>
+      <c r="H19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21">
+        <v>102.7</v>
+      </c>
+      <c r="F21">
+        <v>97.2</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22">
+        <v>89.7</v>
+      </c>
+      <c r="F22">
+        <v>97.2</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="F23">
+        <v>97.2</v>
+      </c>
+      <c r="G23">
+        <v>8.9</v>
+      </c>
+      <c r="H23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24">
+        <v>115.2</v>
+      </c>
+      <c r="F24">
+        <v>94</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" t="s">
+        <v>192</v>
+      </c>
+      <c r="D25">
+        <v>101</v>
+      </c>
+      <c r="F25">
+        <v>94</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+      <c r="H25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26">
+        <v>87.5</v>
+      </c>
+      <c r="F26">
+        <v>94</v>
+      </c>
+      <c r="G26">
+        <v>9</v>
+      </c>
+      <c r="H26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27">
+        <v>78.5</v>
+      </c>
+      <c r="F27">
+        <v>91.1</v>
+      </c>
+      <c r="G27">
+        <v>12</v>
+      </c>
+      <c r="H27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28">
+        <v>121.2</v>
+      </c>
+      <c r="F28">
+        <v>91.1</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29">
+        <v>105.9</v>
+      </c>
+      <c r="F29">
+        <v>91.1</v>
+      </c>
+      <c r="G29">
+        <v>6</v>
+      </c>
+      <c r="H29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30">
+        <v>91.3</v>
+      </c>
+      <c r="F30">
+        <v>91.1</v>
+      </c>
+      <c r="G30">
+        <v>9</v>
+      </c>
+      <c r="H30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31">
+        <v>37.6</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32">
+        <v>117</v>
+      </c>
+      <c r="F32">
+        <v>94.2</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33">
+        <v>102</v>
+      </c>
+      <c r="F33">
+        <v>94.1</v>
+      </c>
+      <c r="G33">
+        <v>6</v>
+      </c>
+      <c r="H33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34">
+        <v>87.9</v>
+      </c>
+      <c r="F34">
+        <v>94.2</v>
+      </c>
+      <c r="G34">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>193</v>
+      </c>
+      <c r="D35">
+        <v>133.19999999999999</v>
+      </c>
+      <c r="F35">
+        <v>91</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" t="s">
+        <v>192</v>
+      </c>
+      <c r="D36">
+        <v>116.5</v>
+      </c>
+      <c r="F36">
+        <v>91</v>
+      </c>
+      <c r="G36">
+        <v>6</v>
+      </c>
+      <c r="H36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" t="s">
+        <v>191</v>
+      </c>
+      <c r="D37">
+        <v>100.6</v>
+      </c>
+      <c r="F37">
+        <v>91</v>
+      </c>
+      <c r="G37">
+        <v>9</v>
+      </c>
+      <c r="H37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38">
+        <v>90.2</v>
+      </c>
+      <c r="F38">
+        <v>88.1</v>
+      </c>
+      <c r="G38">
+        <v>12</v>
+      </c>
+      <c r="H38">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39">
+        <v>140.6</v>
+      </c>
+      <c r="F39">
+        <v>88.1</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40">
+        <v>122.4</v>
+      </c>
+      <c r="F40">
+        <v>88.1</v>
+      </c>
+      <c r="G40">
+        <v>6</v>
+      </c>
+      <c r="H40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41">
+        <v>105.2</v>
+      </c>
+      <c r="F41">
+        <v>88.1</v>
+      </c>
+      <c r="G41">
+        <v>9</v>
+      </c>
+      <c r="H41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42">
+        <v>44.1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43">
+        <v>135.4</v>
+      </c>
+      <c r="F43">
+        <v>91.2</v>
+      </c>
+      <c r="G43">
+        <v>2.9</v>
+      </c>
+      <c r="H43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44">
+        <v>117.6</v>
+      </c>
+      <c r="F44">
+        <v>91.2</v>
+      </c>
+      <c r="G44">
+        <v>6</v>
+      </c>
+      <c r="H44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" t="s">
+        <v>126</v>
+      </c>
+      <c r="D45">
+        <v>101.1</v>
+      </c>
+      <c r="F45">
+        <v>91.2</v>
+      </c>
+      <c r="G45">
+        <v>9</v>
+      </c>
+      <c r="H45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" t="s">
+        <v>193</v>
+      </c>
+      <c r="I46">
+        <v>2.5</v>
+      </c>
+      <c r="J46">
+        <v>3</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>504</v>
+      </c>
+      <c r="M46">
+        <v>504</v>
+      </c>
+      <c r="O46" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" t="s">
+        <v>192</v>
+      </c>
+      <c r="I47">
+        <v>2.5</v>
+      </c>
+      <c r="J47">
+        <v>6</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>442.5</v>
+      </c>
+      <c r="M47">
+        <v>442.5</v>
+      </c>
+      <c r="O47" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" t="s">
+        <v>191</v>
+      </c>
+      <c r="I48">
+        <v>2.5</v>
+      </c>
+      <c r="J48">
+        <v>9</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>383.7</v>
+      </c>
+      <c r="M48">
+        <v>383.7</v>
+      </c>
+      <c r="O48" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>127</v>
+      </c>
+      <c r="C49" t="s">
+        <v>131</v>
+      </c>
+      <c r="I49">
+        <v>-2.5</v>
+      </c>
+      <c r="J49">
+        <v>9</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>344.4</v>
+      </c>
+      <c r="M49">
+        <v>344.4</v>
+      </c>
+      <c r="O49" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" t="s">
+        <v>132</v>
+      </c>
+      <c r="I50">
+        <v>-2.5</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>529.6</v>
+      </c>
+      <c r="M50">
+        <v>529.6</v>
+      </c>
+      <c r="O50" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" t="s">
+        <v>133</v>
+      </c>
+      <c r="I51">
+        <v>-2.5</v>
+      </c>
+      <c r="J51">
+        <v>3</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>463.4</v>
+      </c>
+      <c r="M51">
+        <v>463.4</v>
+      </c>
+      <c r="O51" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" t="s">
+        <v>134</v>
+      </c>
+      <c r="I52">
+        <v>-2.5</v>
+      </c>
+      <c r="J52">
+        <v>6</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>400</v>
+      </c>
+      <c r="M52">
+        <v>400</v>
+      </c>
+      <c r="O52" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" t="s">
+        <v>135</v>
+      </c>
+      <c r="I53">
+        <v>2.5</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>162</v>
+      </c>
+      <c r="M53">
+        <v>162</v>
+      </c>
+      <c r="O53" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" t="s">
+        <v>136</v>
+      </c>
+      <c r="I54">
+        <v>7.5</v>
+      </c>
+      <c r="J54">
+        <v>3</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>511.7</v>
+      </c>
+      <c r="M54">
+        <v>511.7</v>
+      </c>
+      <c r="O54" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" t="s">
+        <v>137</v>
+      </c>
+      <c r="I55">
+        <v>7.5</v>
+      </c>
+      <c r="J55">
+        <v>6</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>446.5</v>
+      </c>
+      <c r="M55">
+        <v>446.5</v>
+      </c>
+      <c r="O55" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" t="s">
+        <v>126</v>
+      </c>
+      <c r="I56">
+        <v>7.5</v>
+      </c>
+      <c r="J56">
+        <v>9</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>385.5</v>
+      </c>
+      <c r="M56">
+        <v>385.5</v>
+      </c>
+      <c r="O56" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3989C9-1A48-4957-A096-E010616680F6}">
+  <dimension ref="A1:AG5"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" t="s">
+        <v>94</v>
+      </c>
+      <c r="P1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S1" t="s">
+        <v>100</v>
+      </c>
+      <c r="T1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U1" t="s">
+        <v>102</v>
+      </c>
+      <c r="V1" t="s">
+        <v>179</v>
+      </c>
+      <c r="W1" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" t="s">
+        <v>195</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K2">
+        <v>157</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>161.69999999999999</v>
+      </c>
+      <c r="O2">
+        <v>100</v>
+      </c>
+      <c r="P2">
+        <v>100</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2">
+        <v>10</v>
+      </c>
+      <c r="S2">
+        <v>10</v>
+      </c>
+      <c r="T2">
+        <v>10</v>
+      </c>
+      <c r="U2">
+        <v>10</v>
+      </c>
+      <c r="V2" t="s">
+        <v>194</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>2.5</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD2">
+        <v>100</v>
+      </c>
+      <c r="AE2">
+        <v>1.6339999999999999</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G3" t="s">
+        <v>195</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" t="s">
+        <v>110</v>
+      </c>
+      <c r="K3">
+        <v>97</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>106.1</v>
+      </c>
+      <c r="O3">
+        <v>100</v>
+      </c>
+      <c r="P3">
+        <v>97</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3">
+        <v>10</v>
+      </c>
+      <c r="S3">
+        <v>10</v>
+      </c>
+      <c r="T3">
+        <v>10</v>
+      </c>
+      <c r="U3">
+        <v>10</v>
+      </c>
+      <c r="V3" t="s">
+        <v>194</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>2.5</v>
+      </c>
+      <c r="AA3">
+        <v>3.02</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD3">
+        <v>100</v>
+      </c>
+      <c r="AE3">
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4">
+        <v>104</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>120.9</v>
+      </c>
+      <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="P4">
+        <v>94</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4">
+        <v>10</v>
+      </c>
+      <c r="S4">
+        <v>10</v>
+      </c>
+      <c r="T4">
+        <v>10</v>
+      </c>
+      <c r="U4">
+        <v>10</v>
+      </c>
+      <c r="V4" t="s">
+        <v>194</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>2.5</v>
+      </c>
+      <c r="AA4">
+        <v>6.02</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD4">
+        <v>100</v>
+      </c>
+      <c r="AE4">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" t="s">
+        <v>110</v>
+      </c>
+      <c r="K5">
+        <v>113</v>
+      </c>
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <v>140.1</v>
+      </c>
+      <c r="O5">
+        <v>100</v>
+      </c>
+      <c r="P5">
+        <v>91</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5">
+        <v>10</v>
+      </c>
+      <c r="S5">
+        <v>10</v>
+      </c>
+      <c r="T5">
+        <v>10</v>
+      </c>
+      <c r="U5">
+        <v>10</v>
+      </c>
+      <c r="V5" t="s">
+        <v>194</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>2.5</v>
+      </c>
+      <c r="AA5">
+        <v>9.02</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD5">
+        <v>100</v>
+      </c>
+      <c r="AE5">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACF7F64-A871-4FEF-9D6A-E7230D8CC25E}">
+  <dimension ref="A1:B58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>188</v>
+      </c>
+      <c r="B32" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>